<commit_message>
Solicitu des gráficas 11_03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion03/Escaleta_CN_11_03_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion03/Escaleta_CN_11_03_CO.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA 10 Y 11\CN_11_03_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado11\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="9435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16605" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="210">
   <si>
     <t>Asignatura</t>
   </si>
@@ -592,12 +592,6 @@
     <t>Motor que incluye preguntas de respuesta abierta del tema La luz y el sonido</t>
   </si>
   <si>
-    <t>¿Qué es el sonido?</t>
-  </si>
-  <si>
-    <t>Rapidez del sonido</t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
@@ -662,6 +656,9 @@
   </si>
   <si>
     <t>Actividad para comprobar el movimiento de las ondas sonoras</t>
+  </si>
+  <si>
+    <t>El  sonido y la luz</t>
   </si>
 </sst>
 </file>
@@ -858,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -930,75 +927,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1043,14 +971,80 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,6 +1139,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1180,6 +1191,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1358,9 +1386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,94 +1416,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="30" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="37" t="s">
+      <c r="N1" s="77"/>
+      <c r="O1" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="59" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="30" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="72"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="60"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1485,7 +1513,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>122</v>
@@ -1502,7 +1530,7 @@
         <v>147</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>147</v>
@@ -1542,14 +1570,12 @@
         <v>123</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>187</v>
-      </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="9"/>
       <c r="G4" s="22" t="s">
         <v>128</v>
@@ -1561,7 +1587,7 @@
         <v>144</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>147</v>
@@ -1601,14 +1627,12 @@
         <v>123</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>188</v>
-      </c>
+      <c r="E5" s="13"/>
       <c r="F5" s="9"/>
       <c r="G5" s="22" t="s">
         <v>129</v>
@@ -1620,7 +1644,7 @@
         <v>144</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>147</v>
@@ -1660,7 +1684,7 @@
         <v>123</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>122</v>
@@ -1677,7 +1701,7 @@
         <v>144</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>144</v>
@@ -1717,7 +1741,7 @@
         <v>123</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>122</v>
@@ -1734,7 +1758,7 @@
         <v>144</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>147</v>
@@ -1766,62 +1790,62 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="73" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+    <row r="8" spans="1:21" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="78" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="79" t="s">
+      <c r="C8" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="E8" s="61" t="s">
-        <v>189</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="63" t="s">
+      <c r="E8" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40" t="s">
         <v>136</v>
       </c>
       <c r="H8" s="21">
         <v>6</v>
       </c>
-      <c r="I8" s="64" t="s">
+      <c r="I8" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="65" t="s">
-        <v>196</v>
-      </c>
-      <c r="K8" s="66" t="s">
+      <c r="J8" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="L8" s="67" t="s">
+      <c r="L8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="62" t="s">
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="P8" s="62" t="s">
+      <c r="P8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="69">
+      <c r="Q8" s="46">
         <v>10</v>
       </c>
-      <c r="R8" s="70" t="s">
+      <c r="R8" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="S8" s="71" t="s">
+      <c r="S8" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="T8" s="72" t="s">
+      <c r="T8" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="U8" s="71" t="s">
+      <c r="U8" s="48" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1833,12 +1857,12 @@
         <v>123</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="58"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="26"/>
       <c r="G9" s="22" t="s">
         <v>149</v>
@@ -1850,7 +1874,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K9" s="24" t="s">
         <v>147</v>
@@ -1890,7 +1914,7 @@
         <v>123</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>148</v>
@@ -1907,7 +1931,7 @@
         <v>144</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>144</v>
@@ -1947,13 +1971,13 @@
         <v>123</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>148</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="22" t="s">
@@ -1966,7 +1990,7 @@
         <v>144</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>144</v>
@@ -1998,62 +2022,62 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="73" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+    <row r="12" spans="1:21" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="78" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="79" t="s">
+      <c r="C12" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="E12" s="61" t="s">
-        <v>189</v>
-      </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="63" t="s">
+      <c r="E12" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40" t="s">
         <v>153</v>
       </c>
       <c r="H12" s="21">
         <v>10</v>
       </c>
-      <c r="I12" s="64" t="s">
+      <c r="I12" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="J12" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="K12" s="66" t="s">
+      <c r="J12" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="K12" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="L12" s="67" t="s">
+      <c r="L12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68" t="s">
+      <c r="M12" s="45"/>
+      <c r="N12" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62" t="s">
+      <c r="O12" s="39"/>
+      <c r="P12" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="74">
+      <c r="Q12" s="51">
         <v>6</v>
       </c>
-      <c r="R12" s="75" t="s">
+      <c r="R12" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="S12" s="76" t="s">
+      <c r="S12" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="T12" s="77" t="s">
+      <c r="T12" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="U12" s="76" t="s">
+      <c r="U12" s="53" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2065,12 +2089,12 @@
         <v>123</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="E13" s="58"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="26"/>
       <c r="G13" s="22" t="s">
         <v>158</v>
@@ -2082,7 +2106,7 @@
         <v>147</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K13" s="24" t="s">
         <v>147</v>
@@ -2122,7 +2146,7 @@
         <v>123</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>157</v>
@@ -2139,7 +2163,7 @@
         <v>144</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>147</v>
@@ -2177,7 +2201,7 @@
         <v>123</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>157</v>
@@ -2196,7 +2220,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>144</v>
@@ -2236,7 +2260,7 @@
         <v>123</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>157</v>
@@ -2253,7 +2277,7 @@
         <v>144</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>144</v>
@@ -2293,13 +2317,13 @@
         <v>123</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>157</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="22" t="s">
@@ -2312,7 +2336,7 @@
         <v>144</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>144</v>
@@ -2344,60 +2368,60 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="73" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="59" t="s">
+    <row r="18" spans="1:21" s="50" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="78" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="80" t="s">
+      <c r="C18" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="61" t="s">
-        <v>189</v>
-      </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="63" t="s">
+      <c r="E18" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40" t="s">
         <v>171</v>
       </c>
       <c r="H18" s="21">
         <v>16</v>
       </c>
-      <c r="I18" s="64" t="s">
+      <c r="I18" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="J18" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="K18" s="66" t="s">
+      <c r="J18" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="K18" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="L18" s="67" t="s">
+      <c r="L18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62" t="s">
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="69" t="s">
+      <c r="Q18" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="R18" s="70">
+      <c r="R18" s="47">
         <v>8</v>
       </c>
-      <c r="S18" s="71" t="s">
+      <c r="S18" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="T18" s="72" t="s">
+      <c r="T18" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="U18" s="71" t="s">
+      <c r="U18" s="48" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2409,12 +2433,12 @@
         <v>123</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="E19" s="58"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="26"/>
       <c r="G19" s="22" t="s">
         <v>173</v>
@@ -2426,7 +2450,7 @@
         <v>144</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K19" s="24" t="s">
         <v>147</v>
@@ -2464,7 +2488,7 @@
         <v>123</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>172</v>
@@ -2472,7 +2496,7 @@
       <c r="E20" s="34"/>
       <c r="F20" s="9"/>
       <c r="G20" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H20" s="21">
         <v>18</v>
@@ -2481,7 +2505,7 @@
         <v>144</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>147</v>
@@ -2519,7 +2543,7 @@
         <v>123</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>177</v>
@@ -2564,7 +2588,7 @@
         <v>123</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>177</v>
@@ -2621,7 +2645,7 @@
         <v>123</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>177</v>
@@ -4117,12 +4141,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4137,12 +4155,18 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>

</xml_diff>